<commit_message>
affichage selectif reglage ok
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDUSCMAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9865936D-AD16-4477-837C-1BD10EA9282B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F437212-9549-4E2D-B0A3-A93277AA4D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05DD1B80-8CFB-4654-8CCA-2DEEC95082EF}"/>
+    <workbookView xWindow="21900" yWindow="480" windowWidth="19190" windowHeight="10070" xr2:uid="{05DD1B80-8CFB-4654-8CCA-2DEEC95082EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="153">
   <si>
     <t>marque</t>
   </si>
@@ -879,14 +879,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5367092F-029D-48C5-9722-8BAB0CEE3785}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,7 +968,7 @@
         <v>2735500</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -993,7 +994,7 @@
         <v>505000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>554500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>2001500</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1149,19 +1150,31 @@
         <v>199000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="C11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>773</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1189,7 +1202,7 @@
         <v>1265000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1215,7 +1228,7 @@
         <v>920500</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -1239,7 +1252,7 @@
         <v>6215500</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1403,7 +1416,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1637,7 +1650,7 @@
         <v>4503500</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1787,7 +1800,7 @@
         <v>1759500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -2265,15 +2278,21 @@
       <c r="C55" s="1">
         <v>2006</v>
       </c>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E55" s="2">
         <v>666</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -2467,15 +2486,21 @@
       <c r="C63" s="1">
         <v>2017</v>
       </c>
-      <c r="D63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E63" s="2">
         <v>676</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="G63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -2529,7 +2554,7 @@
         <v>8970000</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>101</v>
       </c>
@@ -2771,15 +2796,21 @@
       <c r="C75" s="1">
         <v>2018</v>
       </c>
-      <c r="D75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E75" s="2">
         <v>495</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="G75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2895,15 +2926,21 @@
       <c r="C80" s="1">
         <v>2020</v>
       </c>
-      <c r="D80" s="1"/>
+      <c r="D80" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E80" s="2">
         <v>696</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -3081,7 +3118,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>130</v>
       </c>
@@ -3107,7 +3144,7 @@
         <v>266000</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -3143,15 +3180,21 @@
       <c r="C90" s="1">
         <v>2014</v>
       </c>
-      <c r="D90" s="1"/>
+      <c r="D90" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E90" s="2">
         <v>616</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
+      <c r="G90" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
@@ -3205,7 +3248,7 @@
         <v>852000</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>138</v>
       </c>
@@ -3309,7 +3352,7 @@
         <v>1201500</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -3385,7 +3428,7 @@
         <v>205000</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>148</v>
       </c>
@@ -3421,15 +3464,21 @@
       <c r="C101" s="1">
         <v>1972</v>
       </c>
-      <c r="D101" s="1"/>
+      <c r="D101" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E101" s="2">
         <v>176</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
+      <c r="G101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">

</xml_diff>

<commit_message>
supression configreglage + update
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDUSCMAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD68C81-10D1-45CD-93A5-73E0E0FC4FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B7FFF-8B18-4507-959D-FE66B274D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05DD1B80-8CFB-4654-8CCA-2DEEC95082EF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="154">
   <si>
     <t>marque</t>
   </si>
@@ -518,7 +518,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -538,7 +538,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6CAF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -565,6 +565,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -883,7 +886,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,6 +979,9 @@
       <c r="H3" s="1">
         <v>2735500</v>
       </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1147,6 +1153,9 @@
       <c r="H9" s="1">
         <v>362000</v>
       </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1173,6 +1182,9 @@
       <c r="H10" s="1">
         <v>199000</v>
       </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1199,6 +1211,9 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1225,6 +1240,9 @@
       <c r="H12" s="1">
         <v>1265000</v>
       </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1251,6 +1269,9 @@
       <c r="H13" s="1">
         <v>920500</v>
       </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1275,6 +1296,9 @@
       <c r="H14" s="1">
         <v>6215500</v>
       </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1301,6 +1325,9 @@
       <c r="H15" s="1">
         <v>305000</v>
       </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1327,8 +1354,11 @@
       <c r="H16" s="1">
         <v>1604500</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1353,8 +1383,11 @@
       <c r="H17" s="1">
         <v>6376900</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1379,8 +1412,11 @@
       <c r="H18" s="1">
         <v>5516640</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1399,8 +1435,11 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1425,22 +1464,40 @@
       <c r="H20" s="1">
         <v>3901220</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="2">
+        <v>563</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1465,8 +1522,11 @@
       <c r="H22" s="1">
         <v>737000</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1491,8 +1551,11 @@
       <c r="H23" s="1">
         <v>983500</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1517,8 +1580,11 @@
       <c r="H24" s="1">
         <v>858000</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -1543,8 +1609,11 @@
       <c r="H25" s="1">
         <v>880000</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -1569,8 +1638,11 @@
       <c r="H26" s="1">
         <v>11786000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1595,8 +1667,11 @@
       <c r="H27" s="1">
         <v>12030000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1621,8 +1696,11 @@
       <c r="H28" s="1">
         <v>12999500</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -1647,8 +1725,11 @@
       <c r="H29" s="1">
         <v>4369000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1673,8 +1754,11 @@
       <c r="H30" s="1">
         <v>4503500</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1699,8 +1783,11 @@
       <c r="H31" s="1">
         <v>255000</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -1725,8 +1812,11 @@
       <c r="H32" s="1">
         <v>277000</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1736,17 +1826,26 @@
       <c r="C33" s="1">
         <v>2018</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E33" s="2">
         <v>660</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
@@ -1771,8 +1870,11 @@
       <c r="H34" s="1">
         <v>751500</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -1797,8 +1899,11 @@
       <c r="H35" s="1">
         <v>933500</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>62</v>
       </c>
@@ -1823,8 +1928,11 @@
       <c r="H36" s="1">
         <v>1759500</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -1849,8 +1957,11 @@
       <c r="H37" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>69</v>
       </c>
@@ -1875,8 +1986,11 @@
       <c r="H38" s="1">
         <v>1167000</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
@@ -1901,8 +2015,11 @@
       <c r="H39" s="1">
         <v>1429500</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
@@ -1927,8 +2044,11 @@
       <c r="H40" s="1">
         <v>21447500</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
@@ -1953,8 +2073,11 @@
       <c r="H41" s="1">
         <v>1470000</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
@@ -1979,8 +2102,11 @@
       <c r="H42" s="1">
         <v>402500</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
@@ -2005,8 +2131,11 @@
       <c r="H43" s="1">
         <v>1141000</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
@@ -2031,8 +2160,11 @@
       <c r="H44" s="1">
         <v>2401500</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
@@ -2057,8 +2189,11 @@
       <c r="H45" s="1">
         <v>1661500</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>72</v>
       </c>
@@ -2083,8 +2218,11 @@
       <c r="H46" s="1">
         <v>4055000</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>72</v>
       </c>
@@ -2109,8 +2247,11 @@
       <c r="H47" s="1">
         <v>12006000</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -2135,8 +2276,11 @@
       <c r="H48" s="1">
         <v>2501000</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>72</v>
       </c>
@@ -2161,8 +2305,11 @@
       <c r="H49" s="1">
         <v>8100500</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>83</v>
       </c>
@@ -2187,8 +2334,11 @@
       <c r="H50" s="1">
         <v>190000</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
@@ -2213,8 +2363,11 @@
       <c r="H51" s="1">
         <v>236500</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>83</v>
       </c>
@@ -2239,8 +2392,11 @@
       <c r="H52" s="1">
         <v>192500</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>83</v>
       </c>
@@ -2265,8 +2421,11 @@
       <c r="H53" s="1">
         <v>642500</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>83</v>
       </c>
@@ -2291,8 +2450,11 @@
       <c r="H54" s="1">
         <v>1536000</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>83</v>
       </c>
@@ -2317,8 +2479,11 @@
       <c r="H55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>83</v>
       </c>
@@ -2343,8 +2508,11 @@
       <c r="H56" s="1">
         <v>2496500</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>83</v>
       </c>
@@ -2369,8 +2537,11 @@
       <c r="H57" s="1">
         <v>5198240</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>83</v>
       </c>
@@ -2395,8 +2566,11 @@
       <c r="H58" s="1">
         <v>5533740</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>83</v>
       </c>
@@ -2421,8 +2595,11 @@
       <c r="H59" s="1">
         <v>4117665</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>83</v>
       </c>
@@ -2447,8 +2624,11 @@
       <c r="H60" s="1">
         <v>15289000</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>94</v>
       </c>
@@ -2473,8 +2653,11 @@
       <c r="H61" s="1">
         <v>18159500</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>94</v>
       </c>
@@ -2499,8 +2682,11 @@
       <c r="H62" s="1">
         <v>949500</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>94</v>
       </c>
@@ -2525,8 +2711,11 @@
       <c r="H63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>98</v>
       </c>
@@ -2550,6 +2739,9 @@
       </c>
       <c r="H64" s="1">
         <v>9986000</v>
+      </c>
+      <c r="I64">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2577,6 +2769,9 @@
       <c r="H65" s="1">
         <v>8970000</v>
       </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -2661,6 +2856,9 @@
       <c r="H68" s="1">
         <v>2377000</v>
       </c>
+      <c r="I68">
+        <v>7</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -2687,6 +2885,9 @@
       <c r="H69" s="1">
         <v>5027000</v>
       </c>
+      <c r="I69">
+        <v>7</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2713,6 +2914,9 @@
       <c r="H70" s="1">
         <v>2521000</v>
       </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -2737,6 +2941,9 @@
       <c r="H71" s="1">
         <v>10618500</v>
       </c>
+      <c r="I71">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -2763,6 +2970,9 @@
       <c r="H72" s="1">
         <v>2004000</v>
       </c>
+      <c r="I72">
+        <v>7</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -2789,6 +2999,9 @@
       <c r="H73" s="1">
         <v>4407500</v>
       </c>
+      <c r="I73">
+        <v>5</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -2815,6 +3028,9 @@
       <c r="H74" s="1">
         <v>1085000</v>
       </c>
+      <c r="I74">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -2841,6 +3057,9 @@
       <c r="H75" s="1">
         <v>0</v>
       </c>
+      <c r="I75">
+        <v>8</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2867,6 +3086,9 @@
       <c r="H76" s="1">
         <v>553000</v>
       </c>
+      <c r="I76">
+        <v>6</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -2893,6 +3115,9 @@
       <c r="H77" s="1">
         <v>10952000</v>
       </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
@@ -2919,6 +3144,9 @@
       <c r="H78" s="1">
         <v>1268000</v>
       </c>
+      <c r="I78">
+        <v>6</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -2945,6 +3173,9 @@
       <c r="H79" s="1">
         <v>983000</v>
       </c>
+      <c r="I79">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2971,8 +3202,11 @@
       <c r="H80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>121</v>
       </c>
@@ -2997,8 +3231,11 @@
       <c r="H81" s="1">
         <v>1121000</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>121</v>
       </c>
@@ -3023,8 +3260,11 @@
       <c r="H82" s="1">
         <v>1638000</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>121</v>
       </c>
@@ -3049,8 +3289,11 @@
       <c r="H83" s="1">
         <v>3571000</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -3075,8 +3318,11 @@
       <c r="H84" s="1">
         <v>695500</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>127</v>
       </c>
@@ -3101,8 +3347,11 @@
       <c r="H85" s="1">
         <v>1743000</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -3127,8 +3376,11 @@
       <c r="H86" s="1">
         <v>1557500</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>130</v>
       </c>
@@ -3138,17 +3390,26 @@
       <c r="C87" s="1">
         <v>1954</v>
       </c>
-      <c r="D87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E87" s="2">
         <v>337</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G87" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>130</v>
       </c>
@@ -3173,8 +3434,11 @@
       <c r="H88" s="1">
         <v>266000</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -3199,8 +3463,11 @@
       <c r="H89" s="1">
         <v>1674000</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>130</v>
       </c>
@@ -3225,8 +3492,11 @@
       <c r="H90" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>135</v>
       </c>
@@ -3251,8 +3521,11 @@
       <c r="H91" s="1">
         <v>160000</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>135</v>
       </c>
@@ -3277,8 +3550,11 @@
       <c r="H92" s="1">
         <v>852000</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>138</v>
       </c>
@@ -3303,8 +3579,11 @@
       <c r="H93" s="1">
         <v>563999</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>138</v>
       </c>
@@ -3329,8 +3608,11 @@
       <c r="H94" s="1">
         <v>2612000</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>138</v>
       </c>
@@ -3355,8 +3637,11 @@
       <c r="H95" s="1">
         <v>4209500</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>138</v>
       </c>
@@ -3381,8 +3666,11 @@
       <c r="H96" s="1">
         <v>1201500</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -3407,8 +3695,11 @@
       <c r="H97" s="1">
         <v>269500</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>144</v>
       </c>
@@ -3431,8 +3722,11 @@
       <c r="H98" s="1">
         <v>3898000</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>146</v>
       </c>
@@ -3457,8 +3751,11 @@
       <c r="H99" s="1">
         <v>205000</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>148</v>
       </c>
@@ -3483,8 +3780,11 @@
       <c r="H100" s="1">
         <v>22500</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>148</v>
       </c>
@@ -3509,8 +3809,11 @@
       <c r="H101" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>151</v>
       </c>
@@ -3523,7 +3826,7 @@
       <c r="D102" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102" s="4">
         <v>803</v>
       </c>
       <c r="F102" s="3" t="s">
@@ -3534,6 +3837,9 @@
       </c>
       <c r="H102" s="3">
         <v>4334000</v>
+      </c>
+      <c r="I102">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>